<commit_message>
Changed modified sample form fill data
</commit_message>
<xml_diff>
--- a/sample_form_fill_data.xlsx
+++ b/sample_form_fill_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/68ffc9e8a62ebb06/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Git Clone\CA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{B1665FA7-F345-4F9E-B4F9-F7A4E3D4C49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B89A3444-CE80-4918-AB6D-DE5FB37EE99C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05B10D5-6A31-416F-965E-CF0D82DD22C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{60E9B72A-48E4-4FAC-8AB3-722C308DA42D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="3">
   <si>
     <t>address</t>
   </si>
@@ -401,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BAC6B39-EFC0-4861-BE48-307D6DF6E97E}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -423,6 +423,215 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>